<commit_message>
Added functionality to work with different models for context embeddings
</commit_message>
<xml_diff>
--- a/data/data_file.xlsx
+++ b/data/data_file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>antonym_1</t>
   </si>
@@ -68,60 +68,6 @@
   </si>
   <si>
     <t>low temperature</t>
-  </si>
-  <si>
-    <t>big</t>
-  </si>
-  <si>
-    <t>small</t>
-  </si>
-  <si>
-    <t>The elephant is big.</t>
-  </si>
-  <si>
-    <t>The ant is small.</t>
-  </si>
-  <si>
-    <t>large size</t>
-  </si>
-  <si>
-    <t>tiny size</t>
-  </si>
-  <si>
-    <t>fast</t>
-  </si>
-  <si>
-    <t>slow</t>
-  </si>
-  <si>
-    <t>The cheetah runs fast.</t>
-  </si>
-  <si>
-    <t>The snail moves slow.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">high speed </t>
-  </si>
-  <si>
-    <t>low speed</t>
-  </si>
-  <si>
-    <t>good</t>
-  </si>
-  <si>
-    <t>bad</t>
-  </si>
-  <si>
-    <t>Eating healthy food is good for you.</t>
-  </si>
-  <si>
-    <t>Smoking is bad for your health.</t>
-  </si>
-  <si>
-    <t>positive</t>
-  </si>
-  <si>
-    <t>negative</t>
   </si>
 </sst>
 </file>
@@ -468,7 +414,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -542,66 +488,6 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>